<commit_message>
New readme.md; new measurements; one file with a lot of experimental graphics
</commit_message>
<xml_diff>
--- a/measurements2.xlsx
+++ b/measurements2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="15">
   <si>
     <t>distance</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>AC snow</t>
+  </si>
+  <si>
+    <t>half rain half sun</t>
   </si>
 </sst>
 </file>
@@ -251,10 +254,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$190</c:f>
+              <c:f>Sheet1!$A$2:$A$196</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="189"/>
+                <c:ptCount val="195"/>
                 <c:pt idx="0">
                   <c:v>28</c:v>
                 </c:pt>
@@ -821,16 +824,34 @@
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>81.2</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>130.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>67.2</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>43.7</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>56.1</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$190</c:f>
+              <c:f>Sheet1!$B$2:$B$196</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="189"/>
+                <c:ptCount val="195"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1397,6 +1418,24 @@
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1411,11 +1450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442969624"/>
-        <c:axId val="442971976"/>
+        <c:axId val="216164536"/>
+        <c:axId val="393241128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442969624"/>
+        <c:axId val="216164536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -1444,12 +1483,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="442971976"/>
+        <c:crossAx val="393241128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442971976"/>
+        <c:axId val="393241128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,7 +1509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442969624"/>
+        <c:crossAx val="216164536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1523,8 +1562,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I190" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:I190"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I196" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:I196"/>
   <tableColumns count="9">
     <tableColumn id="1" name="distance"/>
     <tableColumn id="2" name="consume"/>
@@ -1827,11 +1866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I190"/>
+  <dimension ref="A1:I196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K194" sqref="K194"/>
+      <selection pane="bottomLeft" activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6865,6 +6904,165 @@
         <v>0</v>
       </c>
       <c r="I190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="B191">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C191">
+        <v>85</v>
+      </c>
+      <c r="D191">
+        <v>22</v>
+      </c>
+      <c r="E191">
+        <v>12</v>
+      </c>
+      <c r="G191" t="s">
+        <v>5</v>
+      </c>
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>67.2</v>
+      </c>
+      <c r="B192">
+        <v>4.3</v>
+      </c>
+      <c r="C192">
+        <v>67</v>
+      </c>
+      <c r="D192">
+        <v>22</v>
+      </c>
+      <c r="E192">
+        <v>18</v>
+      </c>
+      <c r="G192" t="s">
+        <v>5</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>43.7</v>
+      </c>
+      <c r="B193">
+        <v>4.7</v>
+      </c>
+      <c r="C193">
+        <v>44</v>
+      </c>
+      <c r="D193">
+        <v>22</v>
+      </c>
+      <c r="E193">
+        <v>9</v>
+      </c>
+      <c r="F193" t="s">
+        <v>14</v>
+      </c>
+      <c r="G193" t="s">
+        <v>7</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>12.1</v>
+      </c>
+      <c r="B194">
+        <v>4.2</v>
+      </c>
+      <c r="C194">
+        <v>43</v>
+      </c>
+      <c r="D194">
+        <v>22</v>
+      </c>
+      <c r="E194">
+        <v>4</v>
+      </c>
+      <c r="G194" t="s">
+        <v>7</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="I194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>56.1</v>
+      </c>
+      <c r="B195">
+        <v>4.8</v>
+      </c>
+      <c r="C195">
+        <v>82</v>
+      </c>
+      <c r="D195">
+        <v>22</v>
+      </c>
+      <c r="E195">
+        <v>13</v>
+      </c>
+      <c r="G195" t="s">
+        <v>7</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>39</v>
+      </c>
+      <c r="B196">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C196">
+        <v>61</v>
+      </c>
+      <c r="D196">
+        <v>22</v>
+      </c>
+      <c r="E196">
+        <v>16</v>
+      </c>
+      <c r="G196" t="s">
+        <v>7</v>
+      </c>
+      <c r="H196">
+        <v>0</v>
+      </c>
+      <c r="I196">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New measurements Added two files
</commit_message>
<xml_diff>
--- a/measurements2.xlsx
+++ b/measurements2.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="16">
   <si>
     <t>distance</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>half rain half sun</t>
+  </si>
+  <si>
+    <t>sunny</t>
   </si>
 </sst>
 </file>
@@ -254,10 +257,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$196</c:f>
+              <c:f>Sheet1!$A$2:$A$226</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="195"/>
+                <c:ptCount val="225"/>
                 <c:pt idx="0">
                   <c:v>28</c:v>
                 </c:pt>
@@ -842,16 +845,106 @@
                 </c:pt>
                 <c:pt idx="194">
                   <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>28.2</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>19.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>25.9</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>12.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$196</c:f>
+              <c:f>Sheet1!$B$2:$B$226</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="195"/>
+                <c:ptCount val="225"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1436,6 +1529,96 @@
                 </c:pt>
                 <c:pt idx="194">
                   <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1450,11 +1633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216164536"/>
-        <c:axId val="393241128"/>
+        <c:axId val="383178032"/>
+        <c:axId val="383176464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216164536"/>
+        <c:axId val="383178032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -1483,12 +1666,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="393241128"/>
+        <c:crossAx val="383176464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="393241128"/>
+        <c:axId val="383176464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216164536"/>
+        <c:crossAx val="383178032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,12 +1714,12 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>620246</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>356625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>661148</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>56028</xdr:rowOff>
@@ -1562,8 +1745,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I196" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:I196"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I226" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:I226"/>
   <tableColumns count="9">
     <tableColumn id="1" name="distance"/>
     <tableColumn id="2" name="consume"/>
@@ -1866,11 +2049,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I196"/>
+  <dimension ref="A1:I226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D197" sqref="D197"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J225" sqref="J225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7063,6 +7246,792 @@
         <v>0</v>
       </c>
       <c r="I196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>11.8</v>
+      </c>
+      <c r="B197">
+        <v>4.5</v>
+      </c>
+      <c r="C197">
+        <v>41</v>
+      </c>
+      <c r="D197">
+        <v>21.5</v>
+      </c>
+      <c r="E197">
+        <v>13</v>
+      </c>
+      <c r="G197" t="s">
+        <v>7</v>
+      </c>
+      <c r="H197">
+        <v>0</v>
+      </c>
+      <c r="I197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>38.5</v>
+      </c>
+      <c r="B198">
+        <v>4.8</v>
+      </c>
+      <c r="C198">
+        <v>63</v>
+      </c>
+      <c r="D198">
+        <v>21.5</v>
+      </c>
+      <c r="E198">
+        <v>14</v>
+      </c>
+      <c r="G198" t="s">
+        <v>7</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>28.2</v>
+      </c>
+      <c r="B199">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C199">
+        <v>54</v>
+      </c>
+      <c r="D199">
+        <v>21.5</v>
+      </c>
+      <c r="E199">
+        <v>14</v>
+      </c>
+      <c r="G199" t="s">
+        <v>7</v>
+      </c>
+      <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="I199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>2.9</v>
+      </c>
+      <c r="B200">
+        <v>7.4</v>
+      </c>
+      <c r="C200">
+        <v>24</v>
+      </c>
+      <c r="D200">
+        <v>21.5</v>
+      </c>
+      <c r="E200">
+        <v>14</v>
+      </c>
+      <c r="G200" t="s">
+        <v>7</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="I200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>6.1</v>
+      </c>
+      <c r="B201">
+        <v>5.6</v>
+      </c>
+      <c r="C201">
+        <v>24</v>
+      </c>
+      <c r="D201">
+        <v>21.5</v>
+      </c>
+      <c r="E201">
+        <v>13</v>
+      </c>
+      <c r="G201" t="s">
+        <v>7</v>
+      </c>
+      <c r="H201">
+        <v>0</v>
+      </c>
+      <c r="I201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="B202">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C202">
+        <v>43</v>
+      </c>
+      <c r="D202">
+        <v>21.5</v>
+      </c>
+      <c r="E202">
+        <v>13</v>
+      </c>
+      <c r="G202" t="s">
+        <v>7</v>
+      </c>
+      <c r="H202">
+        <v>0</v>
+      </c>
+      <c r="I202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>22.2</v>
+      </c>
+      <c r="B203">
+        <v>3.8</v>
+      </c>
+      <c r="C203">
+        <v>42</v>
+      </c>
+      <c r="E203">
+        <v>15</v>
+      </c>
+      <c r="G203" t="s">
+        <v>7</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="I203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>13.6</v>
+      </c>
+      <c r="B204">
+        <v>4.5</v>
+      </c>
+      <c r="C204">
+        <v>44</v>
+      </c>
+      <c r="D204">
+        <v>19</v>
+      </c>
+      <c r="E204">
+        <v>18</v>
+      </c>
+      <c r="G204" t="s">
+        <v>7</v>
+      </c>
+      <c r="H204">
+        <v>0</v>
+      </c>
+      <c r="I204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>12.6</v>
+      </c>
+      <c r="B205">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C205">
+        <v>33</v>
+      </c>
+      <c r="E205">
+        <v>17</v>
+      </c>
+      <c r="G205" t="s">
+        <v>7</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+      <c r="I205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="B206">
+        <v>5.3</v>
+      </c>
+      <c r="C206">
+        <v>28</v>
+      </c>
+      <c r="D206">
+        <v>22.5</v>
+      </c>
+      <c r="E206">
+        <v>12</v>
+      </c>
+      <c r="F206" t="s">
+        <v>9</v>
+      </c>
+      <c r="G206" t="s">
+        <v>7</v>
+      </c>
+      <c r="H206">
+        <v>1</v>
+      </c>
+      <c r="I206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>7.9</v>
+      </c>
+      <c r="B207">
+        <v>4.7</v>
+      </c>
+      <c r="C207">
+        <v>31</v>
+      </c>
+      <c r="D207">
+        <v>22.5</v>
+      </c>
+      <c r="E207">
+        <v>12</v>
+      </c>
+      <c r="F207" t="s">
+        <v>6</v>
+      </c>
+      <c r="G207" t="s">
+        <v>7</v>
+      </c>
+      <c r="H207">
+        <v>1</v>
+      </c>
+      <c r="I207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>2.4</v>
+      </c>
+      <c r="B208">
+        <v>9</v>
+      </c>
+      <c r="C208">
+        <v>26</v>
+      </c>
+      <c r="D208">
+        <v>20</v>
+      </c>
+      <c r="E208">
+        <v>10</v>
+      </c>
+      <c r="G208" t="s">
+        <v>7</v>
+      </c>
+      <c r="H208">
+        <v>0</v>
+      </c>
+      <c r="I208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B209">
+        <v>6.3</v>
+      </c>
+      <c r="C209">
+        <v>26</v>
+      </c>
+      <c r="D209">
+        <v>20</v>
+      </c>
+      <c r="E209">
+        <v>10</v>
+      </c>
+      <c r="G209" t="s">
+        <v>7</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="I209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B210">
+        <v>3.6</v>
+      </c>
+      <c r="C210">
+        <v>36</v>
+      </c>
+      <c r="D210">
+        <v>20</v>
+      </c>
+      <c r="E210">
+        <v>19</v>
+      </c>
+      <c r="G210" t="s">
+        <v>7</v>
+      </c>
+      <c r="H210">
+        <v>0</v>
+      </c>
+      <c r="I210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>25.9</v>
+      </c>
+      <c r="B211">
+        <v>3.7</v>
+      </c>
+      <c r="C211">
+        <v>39</v>
+      </c>
+      <c r="D211">
+        <v>20</v>
+      </c>
+      <c r="E211">
+        <v>21</v>
+      </c>
+      <c r="G211" t="s">
+        <v>7</v>
+      </c>
+      <c r="H211">
+        <v>0</v>
+      </c>
+      <c r="I211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>1.3</v>
+      </c>
+      <c r="B212">
+        <v>11.5</v>
+      </c>
+      <c r="C212">
+        <v>21</v>
+      </c>
+      <c r="D212">
+        <v>20</v>
+      </c>
+      <c r="E212">
+        <v>10</v>
+      </c>
+      <c r="G212" t="s">
+        <v>7</v>
+      </c>
+      <c r="H212">
+        <v>0</v>
+      </c>
+      <c r="I212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>14.1</v>
+      </c>
+      <c r="B213">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <v>22</v>
+      </c>
+      <c r="D213">
+        <v>20</v>
+      </c>
+      <c r="E213">
+        <v>12</v>
+      </c>
+      <c r="G213" t="s">
+        <v>7</v>
+      </c>
+      <c r="H213">
+        <v>0</v>
+      </c>
+      <c r="I213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>13.4</v>
+      </c>
+      <c r="B214">
+        <v>5.5</v>
+      </c>
+      <c r="C214">
+        <v>31</v>
+      </c>
+      <c r="D214">
+        <v>20</v>
+      </c>
+      <c r="E214">
+        <v>9</v>
+      </c>
+      <c r="G214" t="s">
+        <v>7</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>6.4</v>
+      </c>
+      <c r="B215">
+        <v>4.7</v>
+      </c>
+      <c r="C215">
+        <v>33</v>
+      </c>
+      <c r="D215">
+        <v>20</v>
+      </c>
+      <c r="E215">
+        <v>8</v>
+      </c>
+      <c r="G215" t="s">
+        <v>7</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+      <c r="I215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>12.9</v>
+      </c>
+      <c r="B216">
+        <v>4.5</v>
+      </c>
+      <c r="C216">
+        <v>42</v>
+      </c>
+      <c r="D216">
+        <v>20</v>
+      </c>
+      <c r="E216">
+        <v>13</v>
+      </c>
+      <c r="G216" t="s">
+        <v>7</v>
+      </c>
+      <c r="H216">
+        <v>0</v>
+      </c>
+      <c r="I216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>12.1</v>
+      </c>
+      <c r="B217">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C217">
+        <v>33</v>
+      </c>
+      <c r="D217">
+        <v>22.5</v>
+      </c>
+      <c r="E217">
+        <v>5</v>
+      </c>
+      <c r="G217" t="s">
+        <v>7</v>
+      </c>
+      <c r="H217">
+        <v>0</v>
+      </c>
+      <c r="I217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>15.7</v>
+      </c>
+      <c r="B218">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C218">
+        <v>32</v>
+      </c>
+      <c r="D218">
+        <v>22.5</v>
+      </c>
+      <c r="E218">
+        <v>13</v>
+      </c>
+      <c r="G218" t="s">
+        <v>7</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+      <c r="I218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>16.2</v>
+      </c>
+      <c r="B219">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C219">
+        <v>26</v>
+      </c>
+      <c r="D219">
+        <v>22.5</v>
+      </c>
+      <c r="E219">
+        <v>11</v>
+      </c>
+      <c r="G219" t="s">
+        <v>7</v>
+      </c>
+      <c r="H219">
+        <v>0</v>
+      </c>
+      <c r="I219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>12.8</v>
+      </c>
+      <c r="B220">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C220">
+        <v>22</v>
+      </c>
+      <c r="D220">
+        <v>22.5</v>
+      </c>
+      <c r="E220">
+        <v>12</v>
+      </c>
+      <c r="G220" t="s">
+        <v>7</v>
+      </c>
+      <c r="H220">
+        <v>0</v>
+      </c>
+      <c r="I220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>19</v>
+      </c>
+      <c r="B221">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C221">
+        <v>58</v>
+      </c>
+      <c r="D221">
+        <v>22.5</v>
+      </c>
+      <c r="E221">
+        <v>17</v>
+      </c>
+      <c r="F221" t="s">
+        <v>15</v>
+      </c>
+      <c r="G221" t="s">
+        <v>7</v>
+      </c>
+      <c r="H221">
+        <v>0</v>
+      </c>
+      <c r="I221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>29</v>
+      </c>
+      <c r="B222">
+        <v>4</v>
+      </c>
+      <c r="C222">
+        <v>27</v>
+      </c>
+      <c r="D222">
+        <v>22.5</v>
+      </c>
+      <c r="E222">
+        <v>12</v>
+      </c>
+      <c r="G222" t="s">
+        <v>7</v>
+      </c>
+      <c r="H222">
+        <v>0</v>
+      </c>
+      <c r="I222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>12.1</v>
+      </c>
+      <c r="B223">
+        <v>5</v>
+      </c>
+      <c r="C223">
+        <v>32</v>
+      </c>
+      <c r="D223">
+        <v>22.5</v>
+      </c>
+      <c r="E223">
+        <v>9</v>
+      </c>
+      <c r="G223" t="s">
+        <v>7</v>
+      </c>
+      <c r="H223">
+        <v>0</v>
+      </c>
+      <c r="I223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>12.3</v>
+      </c>
+      <c r="B224">
+        <v>5.2</v>
+      </c>
+      <c r="C224">
+        <v>55</v>
+      </c>
+      <c r="D224">
+        <v>22.5</v>
+      </c>
+      <c r="E224">
+        <v>10</v>
+      </c>
+      <c r="G224" t="s">
+        <v>7</v>
+      </c>
+      <c r="H224">
+        <v>0</v>
+      </c>
+      <c r="I224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>24.8</v>
+      </c>
+      <c r="B225">
+        <v>4</v>
+      </c>
+      <c r="C225">
+        <v>56</v>
+      </c>
+      <c r="D225">
+        <v>22.5</v>
+      </c>
+      <c r="E225">
+        <v>11</v>
+      </c>
+      <c r="G225" t="s">
+        <v>7</v>
+      </c>
+      <c r="H225">
+        <v>0</v>
+      </c>
+      <c r="I225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>12.9</v>
+      </c>
+      <c r="B226">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C226">
+        <v>34</v>
+      </c>
+      <c r="D226">
+        <v>22.5</v>
+      </c>
+      <c r="E226">
+        <v>8</v>
+      </c>
+      <c r="F226" t="s">
+        <v>8</v>
+      </c>
+      <c r="G226" t="s">
+        <v>7</v>
+      </c>
+      <c r="H226">
+        <v>0</v>
+      </c>
+      <c r="I226">
         <v>0</v>
       </c>
     </row>

</xml_diff>